<commit_message>
set valur via excel
</commit_message>
<xml_diff>
--- a/vtiger-crm-fw-a12/src/test/resources/testScriptData.xlsx
+++ b/vtiger-crm-fw-a12/src/test/resources/testScriptData.xlsx
@@ -9,9 +9,22 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bike" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>hello1</t>
+  </si>
+  <si>
+    <t>heyyy</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,195 +435,200 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" t="inlineStr" s="0">
         <is>
           <t>Bike Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" t="inlineStr" s="0">
         <is>
           <t>Engine CC</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="inlineStr" s="0">
         <is>
           <t>Honda CBR500R</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="inlineStr" s="0">
         <is>
           <t>471cc</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr" s="0">
         <is>
           <t>Yamaha R15 V4</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="inlineStr" s="0">
         <is>
           <t>155cc</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="inlineStr" s="0">
         <is>
           <t>KTM Duke 390</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="inlineStr" s="0">
         <is>
           <t>373cc</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="inlineStr" s="0">
         <is>
           <t>Royal Enfield Classic 350</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="inlineStr" s="0">
         <is>
           <t>349cc</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="inlineStr" s="0">
         <is>
           <t>Suzuki Hayabusa</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr" s="0">
         <is>
           <t>1340cc</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="inlineStr" s="0">
         <is>
           <t>BMW G310R</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="inlineStr" s="0">
         <is>
           <t>313cc</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="inlineStr" s="0">
         <is>
           <t>Kawasaki Ninja 650</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="inlineStr" s="0">
         <is>
           <t>649cc</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr" s="0">
         <is>
           <t>TVS Apache RR 310</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="inlineStr" s="0">
         <is>
           <t>312cc</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="inlineStr" s="0">
         <is>
           <t>Ducati Panigale V4</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="inlineStr" s="0">
         <is>
           <t>1103cc</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="inlineStr" s="0">
         <is>
           <t>Harley Davidson Iron 883</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="inlineStr" s="0">
         <is>
           <t>883cc</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="inlineStr" s="0">
         <is>
           <t>Bajaj Pulsar NS200</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="inlineStr" s="0">
         <is>
           <t>199cc</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="inlineStr" s="0">
         <is>
           <t>Triumph Street Triple RS</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="inlineStr" s="0">
         <is>
           <t>765cc</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="inlineStr" s="0">
         <is>
           <t>Kawasaki Z900</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="inlineStr" s="0">
         <is>
           <t>948cc</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="inlineStr" s="0">
         <is>
           <t>Honda Hornet 2.0</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="inlineStr" s="0">
         <is>
           <t>184cc</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="inlineStr" s="0">
         <is>
           <t>Yamaha MT-15</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="inlineStr" s="0">
         <is>
           <t>155cc</t>
         </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="s" s="0">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>